<commit_message>
display table bug fix
</commit_message>
<xml_diff>
--- a/conf/rush.xlsx
+++ b/conf/rush.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="rush" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1698" uniqueCount="855">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1724" uniqueCount="866">
   <si>
     <t>#/*******************************************************************************</t>
   </si>
@@ -2585,6 +2585,39 @@
   </si>
   <si>
     <t>_______\w+(\a</t>
+  </si>
+  <si>
+    <t>#\a)\w+PULM:</t>
+  </si>
+  <si>
+    <t>#\n(P)ULM</t>
+  </si>
+  <si>
+    <t>#\a)\w+IMPRESSION:</t>
+  </si>
+  <si>
+    <t>#\n(I)MPRESSION:</t>
+  </si>
+  <si>
+    <t>#\a)\w+REASON:</t>
+  </si>
+  <si>
+    <t>#\n(R)EASON:</t>
+  </si>
+  <si>
+    <t>#\a)\w+CHEST:</t>
+  </si>
+  <si>
+    <t>#\n(C)HEST:</t>
+  </si>
+  <si>
+    <t>\a)\w+\C\C\C\C+:</t>
+  </si>
+  <si>
+    <t>\n\w+(\C)\C\C\C+:</t>
+  </si>
+  <si>
+    <t>\n(\C)\C\C\C+:</t>
   </si>
 </sst>
 </file>
@@ -2685,18 +2718,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C956"/>
+  <dimension ref="A1:C969"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A934" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B956" activeCellId="0" sqref="B956:C956"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A936" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A970" activeCellId="0" sqref="A970"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="87.4744897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="85.4489795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12018,6 +12051,149 @@
         <v>0</v>
       </c>
       <c r="C956" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="957" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A957" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="B957" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C957" s="0" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="958" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A958" s="0" t="s">
+        <v>856</v>
+      </c>
+      <c r="B958" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C958" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="959" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A959" s="0" t="s">
+        <v>857</v>
+      </c>
+      <c r="B959" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C959" s="0" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="960" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A960" s="0" t="s">
+        <v>858</v>
+      </c>
+      <c r="B960" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C960" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="961" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A961" s="0" t="s">
+        <v>857</v>
+      </c>
+      <c r="B961" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C961" s="0" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="962" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A962" s="0" t="s">
+        <v>858</v>
+      </c>
+      <c r="B962" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C962" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="963" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A963" s="0" t="s">
+        <v>859</v>
+      </c>
+      <c r="B963" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C963" s="0" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="964" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A964" s="0" t="s">
+        <v>860</v>
+      </c>
+      <c r="B964" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C964" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="965" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A965" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="B965" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C965" s="0" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="966" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A966" s="0" t="s">
+        <v>862</v>
+      </c>
+      <c r="B966" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C966" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="967" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A967" s="0" t="s">
+        <v>863</v>
+      </c>
+      <c r="B967" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C967" s="0" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="968" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A968" s="0" t="s">
+        <v>864</v>
+      </c>
+      <c r="B968" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C968" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="969" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A969" s="0" t="s">
+        <v>865</v>
+      </c>
+      <c r="B969" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C969" s="0" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>